<commit_message>
Actualizacion para practica 22
</commit_message>
<xml_diff>
--- a/Practica_2/BB/BB_G1_I.xlsx
+++ b/Practica_2/BB/BB_G1_I.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EUEP2\Git\EUE\Practica_2\BB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC6C83A-0C7E-43D1-B2E3-CED4AC9C98E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E194BAC-3154-4898-A05C-3305418DA63D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E005E2C7-84BE-42EA-AA08-1999F0AD769E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="53">
   <si>
     <t>Material</t>
   </si>
@@ -157,6 +157,42 @@
   </si>
   <si>
     <t>AL</t>
+  </si>
+  <si>
+    <t>it.34</t>
+  </si>
+  <si>
+    <t>it.35</t>
+  </si>
+  <si>
+    <t>it.36</t>
+  </si>
+  <si>
+    <t>it.37</t>
+  </si>
+  <si>
+    <t>it.38</t>
+  </si>
+  <si>
+    <t>it.39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TITANIO </t>
+  </si>
+  <si>
+    <t>ALUMINIO</t>
+  </si>
+  <si>
+    <t>it.40</t>
+  </si>
+  <si>
+    <t>it.41</t>
+  </si>
+  <si>
+    <t>it.42</t>
+  </si>
+  <si>
+    <t>it.43</t>
   </si>
 </sst>
 </file>
@@ -190,7 +226,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -262,6 +298,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF66CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -438,7 +486,7 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -471,6 +519,28 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="43" fontId="0" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="1" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="13" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="43" fontId="0" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="14" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="1" fillId="14" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -522,6 +592,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF66CC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -830,10 +905,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A1D684B-EDD4-45EA-A70A-93E4E99AF29C}">
-  <dimension ref="A1:AE17"/>
+  <dimension ref="A1:AE28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="T24" sqref="T24"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -848,35 +923,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="29"/>
-      <c r="E1" s="30"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="48"/>
       <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="32"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="34" t="s">
+      <c r="H1" s="50"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="37" t="s">
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="38"/>
-      <c r="S1" s="38"/>
-      <c r="T1" s="38"/>
-      <c r="U1" s="39"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="57"/>
     </row>
     <row r="2" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -1302,7 +1377,7 @@
         <v>59.09</v>
       </c>
       <c r="O6" s="24">
-        <f t="shared" ref="O6:O17" si="8">N6-55.32</f>
+        <f t="shared" ref="O6:O25" si="8">N6-55.32</f>
         <v>3.7700000000000031</v>
       </c>
       <c r="P6" s="25">
@@ -1600,31 +1675,21 @@
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="O10" s="19"/>
-      <c r="T10" s="17" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U10" s="26" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="T10" s="17"/>
+      <c r="U10" s="26"/>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A11" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="22"/>
+      <c r="C11" s="39" t="s">
+        <v>47</v>
+      </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
       <c r="O11" s="19"/>
-      <c r="T11" s="17" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U11" s="26" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="T11" s="17"/>
+      <c r="U11" s="26"/>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
@@ -1671,11 +1736,11 @@
       <c r="N12">
         <v>62.91</v>
       </c>
-      <c r="O12" s="19">
+      <c r="O12" s="31">
         <f t="shared" si="8"/>
         <v>7.5899999999999963</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="28">
         <v>150.72999999999999</v>
       </c>
       <c r="Q12" s="15">
@@ -1687,99 +1752,745 @@
       <c r="S12" s="15">
         <v>-187000000</v>
       </c>
-      <c r="T12" s="17">
+      <c r="T12" s="29">
         <f t="shared" si="2"/>
         <v>2.3661057388063504</v>
       </c>
-      <c r="U12" s="26">
+      <c r="U12" s="30">
         <f t="shared" si="5"/>
         <v>2.4657424686750193</v>
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A13" s="14"/>
-      <c r="O13" s="19"/>
+      <c r="A13" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="15">
+        <v>1000000000</v>
+      </c>
+      <c r="E13" s="15">
+        <v>1170000000</v>
+      </c>
+      <c r="F13">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G13">
+        <v>2E-3</v>
+      </c>
+      <c r="H13">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="I13">
+        <f t="shared" ref="I13" si="11">-(F13+H13)/2</f>
+        <v>-2.0500000000000001E-2</v>
+      </c>
+      <c r="J13">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="K13">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L13" s="18">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="M13" s="21">
+        <f t="shared" ref="M13" si="12">-(F13+L13)/2</f>
+        <v>-2.0500000000000001E-2</v>
+      </c>
+      <c r="N13">
+        <v>61.04</v>
+      </c>
+      <c r="O13" s="31">
+        <f t="shared" si="8"/>
+        <v>5.7199999999999989</v>
+      </c>
+      <c r="P13" s="35">
+        <v>157</v>
+      </c>
+      <c r="Q13" s="15">
+        <v>107000000</v>
+      </c>
+      <c r="R13" s="15">
+        <v>220000000</v>
+      </c>
+      <c r="S13" s="15">
+        <v>-228000000</v>
+      </c>
+      <c r="T13" s="29">
+        <f t="shared" ref="T13:T14" si="13">D13/( MAX( Q13:S13)*1.1*1.2*1.1*1.1 ) - 1</f>
+        <v>1.845889397354461</v>
+      </c>
+      <c r="U13" s="30">
+        <f t="shared" ref="U13:U14" si="14">E13/( MAX( Q13:S13)*1.1*1.2*1.1*1.25 ) - 1</f>
+        <v>1.9301277235161534</v>
+      </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="O14" s="19"/>
+      <c r="A14" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="15">
+        <v>999000000</v>
+      </c>
+      <c r="E14" s="15">
+        <v>1103000000</v>
+      </c>
+      <c r="F14">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G14">
+        <v>2E-3</v>
+      </c>
+      <c r="H14">
+        <v>0.04</v>
+      </c>
+      <c r="I14">
+        <f t="shared" ref="I14" si="15">-(F14+H14)/2</f>
+        <v>-2.1500000000000002E-2</v>
+      </c>
+      <c r="J14">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="K14">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L14" s="18">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="M14" s="21">
+        <f t="shared" ref="M14" si="16">-(F14+L14)/2</f>
+        <v>-2.0500000000000001E-2</v>
+      </c>
+      <c r="N14">
+        <v>60.79</v>
+      </c>
+      <c r="O14" s="31">
+        <f t="shared" si="8"/>
+        <v>5.4699999999999989</v>
+      </c>
+      <c r="P14" s="35">
+        <v>150.54</v>
+      </c>
+      <c r="Q14" s="15">
+        <v>91000000</v>
+      </c>
+      <c r="R14" s="15">
+        <v>295000000</v>
+      </c>
+      <c r="S14" s="15">
+        <v>-295000000</v>
+      </c>
+      <c r="T14" s="29">
+        <f t="shared" si="13"/>
+        <v>1.1202358364425877</v>
+      </c>
+      <c r="U14" s="30">
+        <f t="shared" si="14"/>
+        <v>1.0600457580426763</v>
+      </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A15" s="14"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="40"/>
+      <c r="N15" s="35"/>
       <c r="O15" s="19"/>
+      <c r="P15" s="35"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="15"/>
+      <c r="S15" s="41"/>
+      <c r="T15" s="42"/>
+      <c r="U15" s="43"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="14"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="40"/>
+      <c r="N16" s="35"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="35"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="15"/>
+      <c r="S16" s="41"/>
+      <c r="T16" s="42"/>
+      <c r="U16" s="43"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="O17" s="19"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A18" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="O16" s="19"/>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A17" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="C18" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="O18" s="19"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A19" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" t="s">
         <v>23</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C19" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D19" s="15">
         <v>448000000</v>
       </c>
-      <c r="E17" s="15">
+      <c r="E19" s="15">
         <v>523000000</v>
       </c>
-      <c r="F17">
+      <c r="F19">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="G17">
+      <c r="G19">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="H17">
+      <c r="H19">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="I17">
-        <f t="shared" ref="I17" si="11">-(F17+H17)/2</f>
+      <c r="I19">
+        <f t="shared" ref="I19" si="17">-(F19+H19)/2</f>
         <v>-2.4E-2</v>
       </c>
-      <c r="J17">
+      <c r="J19">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="K17">
+      <c r="K19">
         <v>0.02</v>
       </c>
-      <c r="L17" s="18">
+      <c r="L19" s="18">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="M17" s="21">
-        <f t="shared" ref="M17" si="12">-(F17+L17)/2</f>
+      <c r="M19" s="21">
+        <f t="shared" ref="M19" si="18">-(F19+L19)/2</f>
         <v>-2.4E-2</v>
       </c>
-      <c r="N17">
+      <c r="N19">
         <v>61.09</v>
       </c>
-      <c r="O17" s="19">
+      <c r="O19" s="31">
         <f t="shared" si="8"/>
         <v>5.7700000000000031</v>
       </c>
-      <c r="P17">
+      <c r="P19" s="28">
         <v>156</v>
       </c>
-      <c r="Q17" s="15">
+      <c r="Q19" s="15">
         <v>49300000</v>
       </c>
-      <c r="R17" s="15">
+      <c r="R19" s="15">
         <v>118000000</v>
       </c>
-      <c r="S17" s="15">
+      <c r="S19" s="15">
         <v>-118000000</v>
       </c>
-      <c r="T17" s="17">
-        <f t="shared" ref="T17" si="13">D17/( MAX( Q17:S17)*1.1*1.2*1.1*1.1 ) - 1</f>
+      <c r="T19" s="29">
+        <f t="shared" ref="T19:T22" si="19">D19/( MAX( Q19:S19)*1.1*1.2*1.1*1.1 ) - 1</f>
         <v>1.377041177993692</v>
       </c>
-      <c r="U17" s="26">
-        <f t="shared" ref="U17" si="14">E17/( MAX( Q17:S17)*1.1*1.2*1.1*1.25 ) - 1</f>
+      <c r="U19" s="30">
+        <f t="shared" ref="U19:U20" si="20">E19/( MAX( Q19:S19)*1.1*1.2*1.1*1.25 ) - 1</f>
         <v>1.4419853387495913</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A20" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="15">
+        <v>448000000</v>
+      </c>
+      <c r="E20" s="15">
+        <v>523000000</v>
+      </c>
+      <c r="F20">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G20">
+        <v>2E-3</v>
+      </c>
+      <c r="H20">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="I20">
+        <f t="shared" ref="I20" si="21">-(F20+H20)/2</f>
+        <v>-2.4E-2</v>
+      </c>
+      <c r="J20">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="K20">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="L20" s="18">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="M20" s="21">
+        <f t="shared" ref="M20" si="22">-(F20+L20)/2</f>
+        <v>-2.4E-2</v>
+      </c>
+      <c r="N20">
+        <v>59.99</v>
+      </c>
+      <c r="O20" s="31">
+        <f t="shared" si="8"/>
+        <v>4.6700000000000017</v>
+      </c>
+      <c r="P20">
+        <v>154</v>
+      </c>
+      <c r="Q20" s="15">
+        <v>53700000</v>
+      </c>
+      <c r="R20" s="15">
+        <v>137000000</v>
+      </c>
+      <c r="S20" s="15">
+        <v>-137000000</v>
+      </c>
+      <c r="T20" s="29">
+        <f t="shared" si="19"/>
+        <v>1.047378532870479</v>
+      </c>
+      <c r="U20" s="30">
+        <f t="shared" si="20"/>
+        <v>1.1033158392149764</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A21" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="15">
+        <v>448000000</v>
+      </c>
+      <c r="E21" s="15">
+        <v>523000000</v>
+      </c>
+      <c r="F21">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G21">
+        <v>2E-3</v>
+      </c>
+      <c r="H21">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="I21">
+        <f t="shared" ref="I21" si="23">-(F21+H21)/2</f>
+        <v>-2.4E-2</v>
+      </c>
+      <c r="J21">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="K21">
+        <v>0.01</v>
+      </c>
+      <c r="L21" s="18">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="M21" s="21">
+        <f t="shared" ref="M21" si="24">-(F21+L21)/2</f>
+        <v>-2.4E-2</v>
+      </c>
+      <c r="N21">
+        <v>59.62</v>
+      </c>
+      <c r="O21" s="31">
+        <f t="shared" si="8"/>
+        <v>4.2999999999999972</v>
+      </c>
+      <c r="P21">
+        <v>150.28</v>
+      </c>
+      <c r="Q21" s="15">
+        <v>60300000</v>
+      </c>
+      <c r="R21" s="15">
+        <v>165000000</v>
+      </c>
+      <c r="S21" s="15">
+        <v>-165000000</v>
+      </c>
+      <c r="T21" s="29">
+        <f t="shared" si="19"/>
+        <v>0.69994460001973113</v>
+      </c>
+      <c r="U21" s="32">
+        <f>E21/( MAX( Q21:S21)*1.1*1.2*1.1*1.25 ) - 1</f>
+        <v>0.74638951498455586</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A22" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="15">
+        <v>448000000</v>
+      </c>
+      <c r="E22" s="15">
+        <v>523000000</v>
+      </c>
+      <c r="F22">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G22">
+        <v>2E-3</v>
+      </c>
+      <c r="H22">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="I22">
+        <f t="shared" ref="I22" si="25">-(F22+H22)/2</f>
+        <v>-2.5500000000000002E-2</v>
+      </c>
+      <c r="J22">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="K22">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="L22" s="18">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="M22" s="21">
+        <f t="shared" ref="M22" si="26">-(F22+L22)/2</f>
+        <v>-2.5500000000000002E-2</v>
+      </c>
+      <c r="N22">
+        <v>59.62</v>
+      </c>
+      <c r="O22" s="31">
+        <f t="shared" si="8"/>
+        <v>4.2999999999999972</v>
+      </c>
+      <c r="P22">
+        <v>153.96</v>
+      </c>
+      <c r="Q22" s="15">
+        <v>59400000</v>
+      </c>
+      <c r="R22" s="15">
+        <v>166000000</v>
+      </c>
+      <c r="T22" s="29">
+        <f t="shared" si="19"/>
+        <v>0.6897039698991303</v>
+      </c>
+      <c r="U22" s="32">
+        <f t="shared" ref="U22:U25" si="27">E22/( MAX( Q22:S22)*1.1*1.2*1.1*1.25 ) - 1</f>
+        <v>0.73586909621958885</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A23" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="15">
+        <v>448000000</v>
+      </c>
+      <c r="E23" s="15">
+        <v>523000000</v>
+      </c>
+      <c r="F23">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G23">
+        <v>2E-3</v>
+      </c>
+      <c r="H23">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="I23">
+        <f>-(F23+H23)/2</f>
+        <v>-2.5500000000000002E-2</v>
+      </c>
+      <c r="J23">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="K23">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="L23" s="18">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="M23" s="21">
+        <f>-(F23+L23)/2</f>
+        <v>-2.5500000000000002E-2</v>
+      </c>
+      <c r="N23">
+        <v>59.47</v>
+      </c>
+      <c r="O23" s="31">
+        <f>N23-55.32</f>
+        <v>4.1499999999999986</v>
+      </c>
+      <c r="P23">
+        <v>150.91999999999999</v>
+      </c>
+      <c r="Q23" s="15">
+        <v>63400000</v>
+      </c>
+      <c r="R23" s="15">
+        <v>183000000</v>
+      </c>
+      <c r="T23" s="29">
+        <f>D23/( MAX( Q23:S23)*1.1*1.2*1.1*1.1 ) - 1</f>
+        <v>0.53273693444401982</v>
+      </c>
+      <c r="U23" s="32">
+        <f>E23/( MAX( Q23:S23)*1.1*1.2*1.1*1.25 ) - 1</f>
+        <v>0.57461349711722254</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A24" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="41">
+        <v>448000000</v>
+      </c>
+      <c r="E24" s="41">
+        <v>523000000</v>
+      </c>
+      <c r="F24" s="35">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G24" s="35">
+        <v>2E-3</v>
+      </c>
+      <c r="H24" s="35">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="I24" s="35">
+        <f t="shared" ref="I24:I25" si="28">-(F24+H24)/2</f>
+        <v>-2.5500000000000002E-2</v>
+      </c>
+      <c r="J24" s="35">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="K24" s="35">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="L24" s="35">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="M24" s="40">
+        <f t="shared" ref="M24:M25" si="29">-(F24+L24)/2</f>
+        <v>-2.5500000000000002E-2</v>
+      </c>
+      <c r="N24" s="35">
+        <v>59.44</v>
+      </c>
+      <c r="O24" s="19">
+        <f t="shared" si="8"/>
+        <v>4.1199999999999974</v>
+      </c>
+      <c r="P24" s="35">
+        <v>150.03</v>
+      </c>
+      <c r="Q24" s="41">
+        <v>64600000</v>
+      </c>
+      <c r="R24" s="41">
+        <v>188000000</v>
+      </c>
+      <c r="S24" s="35"/>
+      <c r="T24" s="42">
+        <f t="shared" ref="T24:T25" si="30">D24/( MAX( Q24:S24)*1.1*1.2*1.1*1.1 ) - 1</f>
+        <v>0.49197265427263615</v>
+      </c>
+      <c r="U24" s="45">
+        <f t="shared" si="27"/>
+        <v>0.53273547857687098</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="L25" s="35"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A27" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="15">
+        <v>448000000</v>
+      </c>
+      <c r="E27" s="15">
+        <v>523000000</v>
+      </c>
+      <c r="F27">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G27" s="34">
+        <v>2E-3</v>
+      </c>
+      <c r="H27">
+        <v>0.04</v>
+      </c>
+      <c r="I27">
+        <f t="shared" ref="I27" si="31">-(F27+H27)/2</f>
+        <v>-2.1999999999999999E-2</v>
+      </c>
+      <c r="J27">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="K27" s="34">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="L27" s="18">
+        <v>0.04</v>
+      </c>
+      <c r="M27" s="21">
+        <f t="shared" ref="M27" si="32">-(F27+L27)/2</f>
+        <v>-2.1999999999999999E-2</v>
+      </c>
+      <c r="N27">
+        <v>60</v>
+      </c>
+      <c r="O27" s="38">
+        <f t="shared" ref="O27" si="33">N27-55.32</f>
+        <v>4.68</v>
+      </c>
+      <c r="P27" s="34">
+        <v>150.1</v>
+      </c>
+      <c r="Q27" s="15">
+        <v>64600000</v>
+      </c>
+      <c r="R27" s="15">
+        <v>194000000</v>
+      </c>
+      <c r="T27" s="36">
+        <f t="shared" ref="T27" si="34">D27/( MAX( Q27:S27)*1.1*1.2*1.1*1.1 ) - 1</f>
+        <v>0.44582917011987422</v>
+      </c>
+      <c r="U27" s="37">
+        <f t="shared" ref="U27" si="35">E27/( MAX( Q27:S27)*1.1*1.2*1.1*1.25 ) - 1</f>
+        <v>0.4853312885177925</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A28" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="41">
+        <v>448000000</v>
+      </c>
+      <c r="E28" s="41">
+        <v>523000000</v>
+      </c>
+      <c r="F28" s="35">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G28" s="35">
+        <v>2E-3</v>
+      </c>
+      <c r="H28" s="35">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="I28" s="35">
+        <f t="shared" ref="I28" si="36">-(F28+H28)/2</f>
+        <v>-2.2499999999999999E-2</v>
+      </c>
+      <c r="J28" s="35">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="K28" s="35">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="L28" s="35">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="M28" s="40">
+        <f t="shared" ref="M28" si="37">-(F28+L28)/2</f>
+        <v>-2.2499999999999999E-2</v>
+      </c>
+      <c r="N28" s="35">
+        <v>59.44</v>
+      </c>
+      <c r="O28" s="19">
+        <f t="shared" ref="O28" si="38">N28-55.32</f>
+        <v>4.1199999999999974</v>
+      </c>
+      <c r="P28" s="35">
+        <v>150.1</v>
+      </c>
+      <c r="Q28" s="41">
+        <v>64600000</v>
+      </c>
+      <c r="R28" s="41">
+        <v>188000000</v>
+      </c>
+      <c r="S28" s="35"/>
+      <c r="T28" s="42">
+        <f t="shared" ref="T28" si="39">D28/( MAX( Q28:S28)*1.1*1.2*1.1*1.1 ) - 1</f>
+        <v>0.49197265427263615</v>
+      </c>
+      <c r="U28" s="45">
+        <f t="shared" ref="U28" si="40">E28/( MAX( Q28:S28)*1.1*1.2*1.1*1.25 ) - 1</f>
+        <v>0.53273547857687098</v>
       </c>
     </row>
   </sheetData>

</xml_diff>